<commit_message>
procedure de montage du dual lt6105
</commit_message>
<xml_diff>
--- a/montage composants ordre.xlsx
+++ b/montage composants ordre.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guigur/Documents/github/SESAME/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9CEDD5-E199-E242-9F93-415BCF0E4399}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77438E0-BAFE-B641-BBA1-A5E5F1CA234F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{550E6F97-40AB-4C4B-861A-8F315EA1946E}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="116">
   <si>
     <t>1Ω</t>
   </si>
@@ -241,9 +241,6 @@
   </si>
   <si>
     <t>L2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TP1 TP2 TP4 TP7 TP9 TP12 TP13 TP14 TP15 TP16 TP17 TP19 TP20 TP21 TP22 TP23 TP24 TP25 TP26 TP27 TP28 TP29 TP30 TP31 TP32 TP33 TP34 TP36 TP37 TP38 TP42 TP43 TP44 TP45 TP46 TP47 TP48 TP49 </t>
   </si>
   <si>
     <t>Test point</t>
@@ -286,11 +283,6 @@
 R55 </t>
   </si>
   <si>
-    <t xml:space="preserve">R54 
-R58 
-R81 </t>
-  </si>
-  <si>
     <t xml:space="preserve">RShunt1 
 RShunt2 </t>
   </si>
@@ -298,11 +290,6 @@
     <t xml:space="preserve">C8 
 C10 
 C11 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">C3 
-C7 
-C9 </t>
   </si>
   <si>
     <t xml:space="preserve">D3 
@@ -354,14 +341,6 @@
 D22 </t>
   </si>
   <si>
-    <t xml:space="preserve">C50 
-C51 
-C25 
-C35 
-C52 
-C53 </t>
-  </si>
-  <si>
     <t xml:space="preserve">R49 
 R64 </t>
   </si>
@@ -382,12 +361,6 @@
     <t xml:space="preserve">RV1 
 RV2 
 RV3 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">JP15 
-JP16 
-JP17 
-JP18 </t>
   </si>
   <si>
     <t>C36 
@@ -417,17 +390,6 @@
 QRS1</t>
   </si>
   <si>
-    <t>C1 C6 C12 
-C13 C15 C16 
-C17 C19 
-C20 C21 
-C22 C23 
-C24 C26 
-C27 C33 
-C34 C14 
-mod1_C1 mod2_C1</t>
-  </si>
-  <si>
     <t xml:space="preserve">R14 R15 
 R16 R17 
 R18 R19 
@@ -439,26 +401,6 @@
 R75 </t>
   </si>
   <si>
-    <t xml:space="preserve">R3 
-R4 
-R5 
-R22 
-R23 
-R24 
-R25 
-R27 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">R1 R2 R7 
-R26 R29 R31
-R32 R35 R36 
-R37 R40 R50 
-R65 R76 
-R77 R78 
-R84 R97 
-R98 </t>
-  </si>
-  <si>
     <t xml:space="preserve">R44 R45 
 R46 
 R47 
@@ -467,6 +409,68 @@
 R61 
 R62 
 R83 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R54 
+R58 </t>
+  </si>
+  <si>
+    <t>C1 C6 C12 
+C13 C15 C16 
+C17 C20 
+C22 C23 
+C24 C26 
+C27 C33 
+C34 
+mod1_C1 mod2_C1</t>
+  </si>
+  <si>
+    <t>C3 
+C7 
+C9
+C14</t>
+  </si>
+  <si>
+    <t>C50 
+C51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JP10
+JP11 
+JP12 
+JP13
+JP14 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TP1 TP2 TP4 TP7 TP9 TP12 TP13 TP14 TP15 TP16 TP17 TP19 TP21 TP22 TP23 TP24 TP25 TP26 TP27 TP28 TP30 TP31 TP32 TP33 TP34 TP36 TP37 TP38 TP42 TP43 TP44 TP45 TP46 TP47 TP48 TP49 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R3  
+R5 
+R22 
+R23 
+R24 
+R25 
+R27 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R7 R26 R29 
+R31 R32 
+R35 R36 
+R37 R40 
+R50 R65 
+R76 R77 
+R78 R84 
+R97 R98 </t>
+  </si>
+  <si>
+    <t>mod1_U1
+mod1_U2
+mod2_U1
+mod2_U2</t>
+  </si>
+  <si>
+    <t>LT6105</t>
   </si>
 </sst>
 </file>
@@ -498,7 +502,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -565,6 +569,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCFCF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -744,7 +754,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -805,6 +815,8 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -813,6 +825,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFCFCF"/>
       <color rgb="FF70E3FF"/>
       <color rgb="FFFFE370"/>
       <color rgb="FFFFA970"/>
@@ -822,7 +835,6 @@
       <color rgb="FF70B8B8"/>
       <color rgb="FF70B870"/>
       <color rgb="FFB8B870"/>
-      <color rgb="FFB87070"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1135,76 +1147,72 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7EE4DDE-4F65-FE49-A0BB-9559E8A3EAA5}">
   <dimension ref="A1:D90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="25" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80:D90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="192" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="32.5" defaultRowHeight="198" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="8.33203125" style="4"/>
+    <col min="1" max="16384" width="32.5" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="C1" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="C1" s="25" t="s">
+      <c r="D1" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="26" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="27"/>
       <c r="B2" s="28" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C2" s="29" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="30"/>
     </row>
-    <row r="3" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="31"/>
       <c r="B3" s="28" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="32"/>
       <c r="B4" s="28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C4" s="29" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="30"/>
     </row>
-    <row r="5" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33"/>
       <c r="B5" s="28" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D5" s="30"/>
     </row>
-    <row r="6" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="34"/>
       <c r="B6" s="29" t="s">
         <v>2</v>
@@ -1214,7 +1222,7 @@
       </c>
       <c r="D6" s="30"/>
     </row>
-    <row r="7" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="35"/>
       <c r="B7" s="29" t="s">
         <v>4</v>
@@ -1224,7 +1232,7 @@
       </c>
       <c r="D7" s="30"/>
     </row>
-    <row r="8" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="36"/>
       <c r="B8" s="29" t="s">
         <v>6</v>
@@ -1234,7 +1242,7 @@
       </c>
       <c r="D8" s="30"/>
     </row>
-    <row r="9" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="37"/>
       <c r="B9" s="29" t="s">
         <v>8</v>
@@ -1244,19 +1252,19 @@
       </c>
       <c r="D9" s="30"/>
     </row>
-    <row r="10" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="38"/>
       <c r="B10" s="28" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C10" s="29" t="s">
         <v>10</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="192" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="198" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="39"/>
       <c r="B11" s="40" t="s">
         <v>11</v>
@@ -1266,22 +1274,22 @@
       </c>
       <c r="D11" s="41"/>
     </row>
-    <row r="19" spans="1:4" ht="192" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="20" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="198" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="20" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="7" t="s">
         <v>13</v>
@@ -1291,7 +1299,7 @@
       </c>
       <c r="D21" s="8"/>
     </row>
-    <row r="22" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>
       <c r="B22" s="7" t="s">
         <v>15</v>
@@ -1301,7 +1309,7 @@
       </c>
       <c r="D22" s="8"/>
     </row>
-    <row r="23" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="10"/>
       <c r="B23" s="7" t="s">
         <v>17</v>
@@ -1311,98 +1319,98 @@
       </c>
       <c r="D23" s="8"/>
     </row>
-    <row r="24" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11"/>
       <c r="B24" s="6" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="8"/>
     </row>
-    <row r="25" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="12"/>
       <c r="B25" s="6" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>20</v>
       </c>
       <c r="D25" s="8"/>
     </row>
-    <row r="26" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="13"/>
       <c r="B26" s="6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>21</v>
       </c>
       <c r="D26" s="8"/>
     </row>
-    <row r="27" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="14"/>
       <c r="B27" s="6" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>22</v>
       </c>
       <c r="D27" s="8"/>
     </row>
-    <row r="28" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="15"/>
       <c r="B28" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>23</v>
       </c>
       <c r="D28" s="8"/>
     </row>
-    <row r="29" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="16"/>
       <c r="B29" s="6" t="s">
-        <v>84</v>
+        <v>106</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>24</v>
       </c>
       <c r="D29" s="8"/>
     </row>
-    <row r="30" spans="1:4" ht="192" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="198" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="17"/>
       <c r="B30" s="20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C30" s="18" t="s">
         <v>25</v>
       </c>
       <c r="D30" s="19"/>
     </row>
-    <row r="38" spans="1:4" ht="192" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="1:4" ht="192" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="198" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:4" ht="198" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="21"/>
       <c r="B39" s="22"/>
       <c r="C39" s="22"/>
       <c r="D39" s="23"/>
     </row>
-    <row r="40" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="D40" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D40" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="7" t="s">
         <v>26</v>
@@ -1412,17 +1420,17 @@
       </c>
       <c r="D41" s="8"/>
     </row>
-    <row r="42" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="9"/>
       <c r="B42" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>28</v>
       </c>
       <c r="D42" s="8"/>
     </row>
-    <row r="43" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="10"/>
       <c r="B43" s="7" t="s">
         <v>29</v>
@@ -1432,17 +1440,17 @@
       </c>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="11"/>
       <c r="B44" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>31</v>
       </c>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="12"/>
       <c r="B45" s="7" t="s">
         <v>32</v>
@@ -1452,27 +1460,27 @@
       </c>
       <c r="D45" s="8"/>
     </row>
-    <row r="46" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="13"/>
       <c r="B46" s="6" t="s">
-        <v>87</v>
+        <v>108</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>34</v>
       </c>
       <c r="D46" s="8"/>
     </row>
-    <row r="47" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="14"/>
       <c r="B47" s="6" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D47" s="8"/>
     </row>
-    <row r="48" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="15"/>
       <c r="B48" s="7" t="s">
         <v>37</v>
@@ -1484,10 +1492,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="16"/>
       <c r="B49" s="6" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>40</v>
@@ -1496,10 +1504,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="192" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" ht="198" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="17"/>
       <c r="B50" s="20" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C50" s="18" t="s">
         <v>43</v>
@@ -1508,35 +1516,35 @@
         <v>42</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="192" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" ht="198" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="C60" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="D60" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D60" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="5"/>
       <c r="B61" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C61" s="7" t="s">
         <v>36</v>
       </c>
       <c r="D61" s="8"/>
     </row>
-    <row r="62" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="9"/>
       <c r="B62" s="6" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C62" s="7" t="s">
         <v>44</v>
@@ -1545,10 +1553,10 @@
         <v>45</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="10"/>
       <c r="B63" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C63" s="7" t="s">
         <v>46</v>
@@ -1557,7 +1565,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="11"/>
       <c r="B64" s="7" t="s">
         <v>48</v>
@@ -1567,17 +1575,17 @@
       </c>
       <c r="D64" s="8"/>
     </row>
-    <row r="65" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="12"/>
       <c r="B65" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C65" s="7" t="s">
         <v>50</v>
       </c>
       <c r="D65" s="8"/>
     </row>
-    <row r="66" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="13"/>
       <c r="B66" s="7" t="s">
         <v>52</v>
@@ -1587,17 +1595,17 @@
       </c>
       <c r="D66" s="8"/>
     </row>
-    <row r="67" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="14"/>
       <c r="B67" s="6" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C67" s="7" t="s">
         <v>53</v>
       </c>
       <c r="D67" s="8"/>
     </row>
-    <row r="68" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="15"/>
       <c r="B68" s="7" t="s">
         <v>56</v>
@@ -1607,7 +1615,7 @@
       </c>
       <c r="D68" s="8"/>
     </row>
-    <row r="69" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="16"/>
       <c r="B69" s="7" t="s">
         <v>55</v>
@@ -1617,35 +1625,45 @@
       </c>
       <c r="D69" s="8"/>
     </row>
-    <row r="70" spans="1:4" ht="192" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="17"/>
-      <c r="B70" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="C70" s="18" t="s">
+    <row r="70" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="42"/>
+      <c r="B70" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C70" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D70" s="19"/>
-    </row>
-    <row r="79" spans="1:4" ht="192" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="80" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D70" s="8"/>
+    </row>
+    <row r="71" spans="1:4" ht="198" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="43"/>
+      <c r="B71" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="C71" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="D71" s="19"/>
+    </row>
+    <row r="79" spans="1:4" ht="198" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="80" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B80" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="C80" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C80" s="2" t="s">
+      <c r="D80" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D80" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="5"/>
       <c r="B81" s="6" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C81" s="7" t="s">
         <v>59</v>
@@ -1654,10 +1672,10 @@
         <v>60</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="9"/>
       <c r="B82" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C82" s="7" t="s">
         <v>62</v>
@@ -1666,49 +1684,49 @@
         <v>61</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="10"/>
       <c r="B83" s="7" t="s">
         <v>63</v>
       </c>
       <c r="C83" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="D83" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="D83" s="8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="11"/>
       <c r="B84" s="6" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C84" s="7" t="s">
         <v>64</v>
       </c>
       <c r="D84" s="8"/>
     </row>
-    <row r="85" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="12"/>
       <c r="B85" s="6" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C85" s="7" t="s">
         <v>65</v>
       </c>
       <c r="D85" s="8"/>
     </row>
-    <row r="86" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="13"/>
       <c r="B86" s="6" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C86" s="7" t="s">
         <v>66</v>
       </c>
       <c r="D86" s="8"/>
     </row>
-    <row r="87" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="14"/>
       <c r="B87" s="7" t="s">
         <v>67</v>
@@ -1718,17 +1736,17 @@
       </c>
       <c r="D87" s="8"/>
     </row>
-    <row r="88" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="15"/>
       <c r="B88" s="6" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C88" s="7" t="s">
         <v>69</v>
       </c>
       <c r="D88" s="8"/>
     </row>
-    <row r="89" spans="1:4" ht="192" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:4" ht="198" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="16"/>
       <c r="B89" s="7" t="s">
         <v>71</v>
@@ -1738,13 +1756,13 @@
       </c>
       <c r="D89" s="8"/>
     </row>
-    <row r="90" spans="1:4" ht="192" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" ht="198" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="17"/>
       <c r="B90" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="C90" s="18" t="s">
         <v>72</v>
-      </c>
-      <c r="C90" s="18" t="s">
-        <v>73</v>
       </c>
       <c r="D90" s="19"/>
     </row>

</xml_diff>